<commit_message>
Edit `task-3` in `econometrics`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/econometrics/task-3/task-3.xlsx
+++ b/3-course-6-semester/econometrics/task-3/task-3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\econometrics\task-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADF94AC-28F6-48F4-80CE-CAA2F61293F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4C83AD-B1FE-4ACD-AEB3-A25B60DFF485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ДЗ №3" sheetId="1" r:id="rId1"/>
+    <sheet name="Пара" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -43,8 +44,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
   <si>
     <t>y</t>
   </si>
@@ -236,12 +259,108 @@
   <si>
     <t>&lt; 0.05</t>
   </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>X^T</t>
+  </si>
+  <si>
+    <t>X*X^T</t>
+  </si>
+  <si>
+    <t>(X*X^T)^-1</t>
+  </si>
+  <si>
+    <t>X^T*(X*X^T)^-1</t>
+  </si>
+  <si>
+    <t>X^T*(X*X^T)^-1*X</t>
+  </si>
+  <si>
+    <t>(1+…)^0,5</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>Интервальный прогноз</t>
+  </si>
+  <si>
+    <t>Точечный прогноз</t>
+  </si>
+  <si>
+    <t>Строим матрицу</t>
+  </si>
+  <si>
+    <t>Определитель</t>
+  </si>
+  <si>
+    <t xml:space="preserve">а = </t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>A парам</t>
+  </si>
+  <si>
+    <t>B1 парам</t>
+  </si>
+  <si>
+    <t>B2 парам</t>
+  </si>
+  <si>
+    <t>Показатели</t>
+  </si>
+  <si>
+    <t>delta r11</t>
+  </si>
+  <si>
+    <t>delta r</t>
+  </si>
+  <si>
+    <t>R^2</t>
+  </si>
+  <si>
+    <t>adj R^2</t>
+  </si>
+  <si>
+    <t>n=10</t>
+  </si>
+  <si>
+    <t>beta1</t>
+  </si>
+  <si>
+    <t>d beta1</t>
+  </si>
+  <si>
+    <t>d beta2</t>
+  </si>
+  <si>
+    <t>beta2</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +392,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -294,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -567,11 +693,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -590,33 +805,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -645,8 +833,76 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -749,8 +1005,8 @@
       <xdr:row>23</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -843,7 +1099,7 @@
                         <a:schemeClr val="dk1"/>
                       </a:solidFill>
                       <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
@@ -890,7 +1146,7 @@
                         <a:schemeClr val="dk1"/>
                       </a:solidFill>
                       <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
@@ -902,7 +1158,7 @@
                         <a:schemeClr val="dk1"/>
                       </a:solidFill>
                       <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
@@ -916,7 +1172,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -929,7 +1185,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -943,7 +1199,7 @@
                             <a:schemeClr val="dk1"/>
                           </a:solidFill>
                           <a:effectLst/>
-                          <a:latin typeface="+mn-lt"/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                           <a:ea typeface="+mn-ea"/>
                           <a:cs typeface="+mn-cs"/>
                         </a:rPr>
@@ -1067,7 +1323,7 @@
                         <a:schemeClr val="dk1"/>
                       </a:solidFill>
                       <a:effectLst/>
-                      <a:latin typeface="+mn-lt"/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
@@ -1106,7 +1362,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="TextBox 2">
@@ -1279,6 +1535,1250 @@
         </xdr:sp>
       </mc:Fallback>
     </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>264584</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>52918</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>349250</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>105834</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30580EF8-8465-4A07-9938-261F2C4A9CD0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="264584" y="10498668"/>
+              <a:ext cx="4381499" cy="444499"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>𝑦</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>=7.56</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>−</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="ru-RU" sz="1400" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>4.67</m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑥</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>1</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                  <m:r>
+                    <a:rPr lang="ru-RU" sz="1400" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>+0.19</m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>𝑥</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                          <a:solidFill>
+                            <a:schemeClr val="dk1"/>
+                          </a:solidFill>
+                          <a:effectLst/>
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:rPr>
+                        <m:t>2</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1"/>
+                      </a:solidFill>
+                      <a:effectLst/>
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:rPr>
+                    <m:t>−</m:t>
+                  </m:r>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>уравнение регрессии</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30580EF8-8465-4A07-9938-261F2C4A9CD0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="264584" y="10498668"/>
+              <a:ext cx="4381499" cy="444499"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:ln/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="dk1"/>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="lt1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="dk1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr/>
+              </a:pPr>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑦=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>7.56</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>4.67</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑥_1</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>+0.19</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400" b="0" i="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>𝑥_2−</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="ru-RU" sz="1400">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:rPr>
+                <a:t>уравнение регрессии</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1400">
+                <a:effectLst/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>607483</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>27517</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>593725</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>170392</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{419F92D8-DFBC-494A-8811-C432911BBCC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3676650" y="228600"/>
+          <a:ext cx="4156075" cy="343959"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Найти уравнение регрессии</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> со значимыми параметрами</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>455084</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>42333</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>10583</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FABA5217-9343-431C-8D53-07E37458DABE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1068917" y="11874500"/>
+          <a:ext cx="4275666" cy="518583"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Дать</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> точечный прогноз </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>x1 = 1; x2=7</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Дать интервальный прогноз</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24355991-6D93-4AA8-A668-0AD78AD1791D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4010025" y="361950"/>
+          <a:ext cx="6029325" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Изучается зависимость</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> прибыли </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>y </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>от </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> x1 - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>кол-во выпущенной продукции и </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>x2 - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>процент простоев оборудования</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Система нормальных уравнений составила</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>10</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>a+123b1+138b2 = 161</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>123a+1635b1+1591b2 = 2120</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>138a+1591b1+2048b2 = 2082</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Требуется найти уравнение регрессии</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171451</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F0D4705-E230-43DB-80CC-838EFF54616C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6057901" y="2162175"/>
+          <a:ext cx="2076449" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>y = 10.73 + 0.8346x1 - 0.355x2</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD8F54D1-DC9C-411E-AB05-7ECB0F1BDDF6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3829050" y="6800850"/>
+          <a:ext cx="6029325" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Найти коэффициент</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> детерминации по модели, если известны парные коэффициенты корреляции</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Ryx1 = 0.956</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Ryx2 = </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>-</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>0.882</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Rx1x2 = -0.803</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Найти нормированный коэффициент детерминации</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AB9483C-85F3-4790-88D2-639C0F5F39F3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5743575" y="9705975"/>
+          <a:ext cx="6638925" cy="1228725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="1" i="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>ДЗ</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Найти уравнение регрессии</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> в стандартизованном масштабе -</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Найти частные коэффициенты корреляции</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Найти коэффициенты эластичности</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Дать точечный прогноз при </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>x1 = 20, x2 = 7</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>Дать интервальный прогноз учитывая что стандартная ошибка регрессии равна 1.111665</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93C7F373-73B3-4833-B515-56E085852349}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4667251" y="11372850"/>
+          <a:ext cx="3971924" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>t_Y = beta_1*t_X1 + beta_2*t_X2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>0.956 = beta_1 - 0.803*beta_2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>-0.882 = -0.803 + beta_2</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="TextBox 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B4090F5-F39B-41E3-8595-1B215B9DEA51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6496051" y="14049375"/>
+          <a:ext cx="2533649" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0">
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>t_Y = 0.697523*t_X1 - 0.32189*t_X2</a:t>
+          </a:r>
+          <a:endParaRPr lang="ru-RU" sz="1200" b="0" i="1" baseline="0">
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1547,14 +3047,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:R41"/>
+  <dimension ref="B1:R104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
     <col min="12" max="12" width="23" customWidth="1"/>
@@ -1568,30 +3070,30 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="12" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="16">
+      <c r="B3" s="7">
         <v>4</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="8">
         <v>1</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="8">
         <v>8</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="9">
         <v>24</v>
       </c>
     </row>
@@ -1695,80 +3197,80 @@
       <c r="E10" s="6">
         <v>28</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="25"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="J11" s="22" t="s">
+      <c r="J11" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="K11" s="22">
+      <c r="K11" s="13">
         <v>0.96467046096630127</v>
       </c>
     </row>
     <row r="12" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="13">
         <v>0.93058909826093628</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-      <c r="J13" s="22" t="s">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="J13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="K13" s="22">
+      <c r="K13" s="13">
         <v>0.8785309219566384</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="J14" s="22" t="s">
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="24"/>
+      <c r="J14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="22">
+      <c r="K14" s="13">
         <v>0.26440460017804762</v>
       </c>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="12"/>
-      <c r="J15" s="23" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="24"/>
+      <c r="J15" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="14">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="26"/>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
@@ -1776,214 +3278,214 @@
       </c>
     </row>
     <row r="18" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J18" s="24"/>
-      <c r="K18" s="24" t="s">
+      <c r="J18" s="15"/>
+      <c r="K18" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="L18" s="24" t="s">
+      <c r="L18" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M18" s="24" t="s">
+      <c r="M18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N18" s="24" t="s">
+      <c r="N18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="O18" s="24" t="s">
+      <c r="O18" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J19" s="22" t="s">
+      <c r="J19" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="22">
+      <c r="K19" s="13">
         <v>3</v>
       </c>
-      <c r="L19" s="22">
+      <c r="L19" s="13">
         <v>3.7491108296187465</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="13">
         <v>1.2497036098729155</v>
       </c>
-      <c r="N19" s="22">
+      <c r="N19" s="13">
         <v>17.87594503544123</v>
       </c>
-      <c r="O19" s="22">
+      <c r="O19" s="13">
         <v>8.8217058025190503E-3</v>
       </c>
     </row>
     <row r="20" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J20" s="22" t="s">
+      <c r="J20" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="13">
         <v>4</v>
       </c>
-      <c r="L20" s="22">
+      <c r="L20" s="13">
         <v>0.27963917038125291</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="13">
         <v>6.9909792595313228E-2</v>
       </c>
-      <c r="N20" s="22"/>
-      <c r="O20" s="22"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
     </row>
     <row r="21" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="14">
         <v>7</v>
       </c>
-      <c r="L21" s="23">
+      <c r="L21" s="14">
         <v>4.0287499999999996</v>
       </c>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="14"/>
     </row>
     <row r="22" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J23" s="24"/>
-      <c r="K23" s="24" t="s">
+      <c r="J23" s="15"/>
+      <c r="K23" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="L23" s="24" t="s">
+      <c r="L23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="M23" s="24" t="s">
+      <c r="M23" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="24" t="s">
+      <c r="N23" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="O23" s="24" t="s">
+      <c r="O23" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="P23" s="24" t="s">
+      <c r="P23" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="Q23" s="24" t="s">
+      <c r="Q23" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="R23" s="24" t="s">
+      <c r="R23" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J24" s="22" t="s">
+      <c r="J24" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="K24" s="22">
+      <c r="K24" s="13">
         <v>9.8059923092761672</v>
       </c>
-      <c r="L24" s="22">
+      <c r="L24" s="13">
         <v>2.5713953251402275</v>
       </c>
-      <c r="M24" s="22">
+      <c r="M24" s="13">
         <v>3.8134907586570379</v>
       </c>
-      <c r="N24" s="26">
+      <c r="N24" s="17">
         <v>1.8883454749252866E-2</v>
       </c>
-      <c r="O24" s="22">
+      <c r="O24" s="13">
         <v>2.6666543452620939</v>
       </c>
-      <c r="P24" s="22">
+      <c r="P24" s="13">
         <v>16.945330273290239</v>
       </c>
-      <c r="Q24" s="22">
+      <c r="Q24" s="13">
         <v>2.6666543452620939</v>
       </c>
-      <c r="R24" s="22">
+      <c r="R24" s="13">
         <v>16.945330273290239</v>
       </c>
     </row>
     <row r="25" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J25" s="22" t="s">
+      <c r="J25" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="22">
+      <c r="K25" s="13">
         <v>-5.9543453702621605</v>
       </c>
-      <c r="L25" s="22">
+      <c r="L25" s="13">
         <v>1.6738367210180165</v>
       </c>
-      <c r="M25" s="22">
+      <c r="M25" s="13">
         <v>-3.5573035861232429</v>
       </c>
-      <c r="N25" s="26">
+      <c r="N25" s="17">
         <v>2.36431244336422E-2</v>
       </c>
-      <c r="O25" s="22">
+      <c r="O25" s="13">
         <v>-10.601661141232956</v>
       </c>
-      <c r="P25" s="22">
+      <c r="P25" s="13">
         <v>-1.3070295992913641</v>
       </c>
-      <c r="Q25" s="22">
+      <c r="Q25" s="13">
         <v>-10.601661141232956</v>
       </c>
-      <c r="R25" s="22">
+      <c r="R25" s="13">
         <v>-1.3070295992913641</v>
       </c>
     </row>
     <row r="26" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J26" s="22" t="s">
+      <c r="J26" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="13">
         <v>0.18270087981435415</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="13">
         <v>7.2358383398542489E-2</v>
       </c>
-      <c r="M26" s="22">
+      <c r="M26" s="13">
         <v>2.524944190751977</v>
       </c>
-      <c r="N26" s="27">
+      <c r="N26" s="28">
         <v>6.5013524286557031E-2</v>
       </c>
-      <c r="O26" s="22">
+      <c r="O26" s="13">
         <v>-1.819819959255442E-2</v>
       </c>
-      <c r="P26" s="22">
+      <c r="P26" s="13">
         <v>0.38359995922126272</v>
       </c>
-      <c r="Q26" s="22">
+      <c r="Q26" s="13">
         <v>-1.819819959255442E-2</v>
       </c>
-      <c r="R26" s="22">
+      <c r="R26" s="13">
         <v>0.38359995922126272</v>
       </c>
     </row>
     <row r="27" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J27" s="23" t="s">
+      <c r="J27" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="K27" s="23">
+      <c r="K27" s="14">
         <v>-3.9000651096011564E-2</v>
       </c>
-      <c r="L27" s="23">
+      <c r="L27" s="14">
         <v>3.533874398505029E-2</v>
       </c>
-      <c r="M27" s="23">
+      <c r="M27" s="14">
         <v>-1.1036230125357711</v>
       </c>
-      <c r="N27" s="28">
+      <c r="N27" s="18">
         <v>0.33168291438885578</v>
       </c>
-      <c r="O27" s="23">
+      <c r="O27" s="14">
         <v>-0.1371167338571424</v>
       </c>
-      <c r="P27" s="23">
+      <c r="P27" s="14">
         <v>5.9115431665119282E-2</v>
       </c>
-      <c r="Q27" s="23">
+      <c r="Q27" s="14">
         <v>-0.1371167338571424</v>
       </c>
-      <c r="R27" s="23">
+      <c r="R27" s="14">
         <v>5.9115431665119282E-2</v>
       </c>
     </row>
@@ -1999,112 +3501,1042 @@
     </row>
     <row r="32" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J33" s="24" t="s">
+      <c r="J33" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="K33" s="24" t="s">
+      <c r="K33" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="L33" s="24" t="s">
+      <c r="L33" s="15" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J34" s="22">
+      <c r="J34" s="13">
         <v>1</v>
       </c>
-      <c r="K34" s="22">
+      <c r="K34" s="13">
         <v>4.3772383512245625</v>
       </c>
-      <c r="L34" s="22">
+      <c r="L34" s="13">
         <v>-0.37723835122456251</v>
       </c>
     </row>
     <row r="35" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J35" s="22">
+      <c r="J35" s="13">
         <v>2</v>
       </c>
-      <c r="K35" s="22">
+      <c r="K35" s="13">
         <v>5.0773724658731085</v>
       </c>
-      <c r="L35" s="22">
+      <c r="L35" s="13">
         <v>0.12262753412689165</v>
       </c>
     </row>
     <row r="36" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J36" s="22">
+      <c r="J36" s="13">
         <v>3</v>
       </c>
-      <c r="K36" s="22">
+      <c r="K36" s="13">
         <v>3.5724046589536842</v>
       </c>
-      <c r="L36" s="22">
+      <c r="L36" s="13">
         <v>0.22759534104631562</v>
       </c>
     </row>
     <row r="37" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J37" s="22">
+      <c r="J37" s="13">
         <v>4</v>
       </c>
-      <c r="K37" s="22">
+      <c r="K37" s="13">
         <v>2.8722705443051373</v>
       </c>
-      <c r="L37" s="22">
+      <c r="L37" s="13">
         <v>2.7729455694862626E-2</v>
       </c>
     </row>
     <row r="38" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J38" s="22">
+      <c r="J38" s="13">
         <v>5</v>
       </c>
-      <c r="K38" s="22">
+      <c r="K38" s="13">
         <v>4.6482573443073623</v>
       </c>
-      <c r="L38" s="22">
+      <c r="L38" s="13">
         <v>-4.8257344307362615E-2</v>
       </c>
     </row>
     <row r="39" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J39" s="22">
+      <c r="J39" s="13">
         <v>6</v>
       </c>
-      <c r="K39" s="22">
+      <c r="K39" s="13">
         <v>4.3732672220460005</v>
       </c>
-      <c r="L39" s="22">
+      <c r="L39" s="13">
         <v>0.12673277795399951</v>
       </c>
     </row>
     <row r="40" spans="10:12" x14ac:dyDescent="0.25">
-      <c r="J40" s="22">
+      <c r="J40" s="13">
         <v>7</v>
       </c>
-      <c r="K40" s="22">
+      <c r="K40" s="13">
         <v>3.8948346383078194</v>
       </c>
-      <c r="L40" s="22">
+      <c r="L40" s="13">
         <v>-0.19483463830781922</v>
       </c>
     </row>
     <row r="41" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J41" s="23">
+      <c r="J41" s="14">
         <v>8</v>
       </c>
-      <c r="K41" s="23">
+      <c r="K41" s="14">
         <v>4.8843547749823326</v>
       </c>
-      <c r="L41" s="23">
+      <c r="L41" s="14">
         <v>0.11564522501766739</v>
       </c>
     </row>
+    <row r="47" spans="10:12" x14ac:dyDescent="0.25">
+      <c r="J47" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="10:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="49" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J49" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K49" s="16"/>
+    </row>
+    <row r="50" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J50" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="K50" s="13">
+        <v>0.95365285119757537</v>
+      </c>
+    </row>
+    <row r="51" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J51" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="K51" s="13">
+        <v>0.90945376059726479</v>
+      </c>
+    </row>
+    <row r="52" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J52" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K52" s="13">
+        <v>0.87323526483617075</v>
+      </c>
+    </row>
+    <row r="53" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J53" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="K53" s="13">
+        <v>0.27010670557902461</v>
+      </c>
+    </row>
+    <row r="54" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J54" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K54" s="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J56" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J57" s="15"/>
+      <c r="K57" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="L57" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="M57" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N57" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O57" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J58" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="K58" s="13">
+        <v>2</v>
+      </c>
+      <c r="L58" s="13">
+        <v>3.6639618380062302</v>
+      </c>
+      <c r="M58" s="13">
+        <v>1.8319809190031151</v>
+      </c>
+      <c r="N58" s="13">
+        <v>25.110202439003562</v>
+      </c>
+      <c r="O58" s="13">
+        <v>2.4670391666680282E-3</v>
+      </c>
+    </row>
+    <row r="59" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J59" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="K59" s="13">
+        <v>5</v>
+      </c>
+      <c r="L59" s="13">
+        <v>0.36478816199376946</v>
+      </c>
+      <c r="M59" s="13">
+        <v>7.2957632398753886E-2</v>
+      </c>
+      <c r="N59" s="13"/>
+      <c r="O59" s="13"/>
+    </row>
+    <row r="60" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J60" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="K60" s="14">
+        <v>7</v>
+      </c>
+      <c r="L60" s="14">
+        <v>4.0287499999999996</v>
+      </c>
+      <c r="M60" s="14"/>
+      <c r="N60" s="14"/>
+      <c r="O60" s="14"/>
+    </row>
+    <row r="61" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J62" s="15"/>
+      <c r="K62" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="L62" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="M62" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N62" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O62" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P62" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q62" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="R62" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J63" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="K63" s="13">
+        <v>7.5609034267912776</v>
+      </c>
+      <c r="L63" s="13">
+        <v>1.6067316214697069</v>
+      </c>
+      <c r="M63" s="13">
+        <v>4.7057662435716425</v>
+      </c>
+      <c r="N63" s="13">
+        <v>5.3096667401669436E-3</v>
+      </c>
+      <c r="O63" s="13">
+        <v>3.4306683058987657</v>
+      </c>
+      <c r="P63" s="13">
+        <v>11.691138547683789</v>
+      </c>
+      <c r="Q63" s="13">
+        <v>3.4306683058987657</v>
+      </c>
+      <c r="R63" s="13">
+        <v>11.691138547683789</v>
+      </c>
+    </row>
+    <row r="64" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J64" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="K64" s="13">
+        <v>-4.673520249221184</v>
+      </c>
+      <c r="L64" s="13">
+        <v>1.2321712776211875</v>
+      </c>
+      <c r="M64" s="13">
+        <v>-3.7929144544286215</v>
+      </c>
+      <c r="N64" s="13">
+        <v>1.2720393136539701E-2</v>
+      </c>
+      <c r="O64" s="13">
+        <v>-7.8409173538669998</v>
+      </c>
+      <c r="P64" s="13">
+        <v>-1.5061231445753682</v>
+      </c>
+      <c r="Q64" s="13">
+        <v>-7.8409173538669998</v>
+      </c>
+      <c r="R64" s="13">
+        <v>-1.5061231445753682</v>
+      </c>
+    </row>
+    <row r="65" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J65" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K65" s="14">
+        <v>0.18598130841121499</v>
+      </c>
+      <c r="L65" s="14">
+        <v>7.3856457091526148E-2</v>
+      </c>
+      <c r="M65" s="14">
+        <v>2.5181455452261789</v>
+      </c>
+      <c r="N65" s="14">
+        <v>5.3295163293457785E-2</v>
+      </c>
+      <c r="O65" s="14">
+        <v>-3.8727586327150232E-3</v>
+      </c>
+      <c r="P65" s="14">
+        <v>0.375835375455145</v>
+      </c>
+      <c r="Q65" s="14">
+        <v>-3.8727586327150232E-3</v>
+      </c>
+      <c r="R65" s="14">
+        <v>0.375835375455145</v>
+      </c>
+    </row>
+    <row r="69" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J69" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B70" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C70" s="48">
+        <f>K63+K64*1+K65*7</f>
+        <v>4.1892523364485985</v>
+      </c>
+    </row>
+    <row r="71" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J71" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="K71" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L71" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J72" s="13">
+        <v>1</v>
+      </c>
+      <c r="K72" s="13">
+        <v>4.3752336448598133</v>
+      </c>
+      <c r="L72" s="13">
+        <v>-0.37523364485981325</v>
+      </c>
+    </row>
+    <row r="73" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J73" s="13">
+        <v>2</v>
+      </c>
+      <c r="K73" s="13">
+        <v>5.0285669781931475</v>
+      </c>
+      <c r="L73" s="13">
+        <v>0.17143302180685271</v>
+      </c>
+    </row>
+    <row r="74" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J74" s="13">
+        <v>3</v>
+      </c>
+      <c r="K74" s="13">
+        <v>3.5359190031152652</v>
+      </c>
+      <c r="L74" s="13">
+        <v>0.26408099688473463</v>
+      </c>
+    </row>
+    <row r="75" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>37</v>
+      </c>
+      <c r="C75">
+        <f>K53</f>
+        <v>0.27010670557902461</v>
+      </c>
+      <c r="J75" s="13">
+        <v>4</v>
+      </c>
+      <c r="K75" s="13">
+        <v>2.8825856697819323</v>
+      </c>
+      <c r="L75" s="13">
+        <v>1.7414330218067597E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76">
+        <f>C75*L104</f>
+        <v>0.28664013558392137</v>
+      </c>
+      <c r="J76" s="13">
+        <v>5</v>
+      </c>
+      <c r="K76" s="13">
+        <v>4.4229283489096582</v>
+      </c>
+      <c r="L76" s="13">
+        <v>0.1770716510903414</v>
+      </c>
+    </row>
+    <row r="77" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="J77" s="13">
+        <v>6</v>
+      </c>
+      <c r="K77" s="13">
+        <v>4.4706230529595024</v>
+      </c>
+      <c r="L77" s="13">
+        <v>2.9376947040497647E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>47</v>
+      </c>
+      <c r="C78">
+        <f>_xlfn.T.INV.2T(0.05,K59)</f>
+        <v>2.570581835636315</v>
+      </c>
+      <c r="J78" s="13">
+        <v>7</v>
+      </c>
+      <c r="K78" s="13">
+        <v>4.0032710280373838</v>
+      </c>
+      <c r="L78" s="13">
+        <v>-0.30327102803738359</v>
+      </c>
+    </row>
+    <row r="79" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>46</v>
+      </c>
+      <c r="C79">
+        <f>C76*C78</f>
+        <v>0.73683192589635882</v>
+      </c>
+      <c r="J79" s="14">
+        <v>8</v>
+      </c>
+      <c r="K79" s="14">
+        <v>4.9808722741433034</v>
+      </c>
+      <c r="L79" s="14">
+        <v>1.9127725856696642E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B80" s="56" t="s">
+        <v>48</v>
+      </c>
+      <c r="C80" s="57"/>
+    </row>
+    <row r="81" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="58">
+        <f>C70-C79</f>
+        <v>3.4524204105522398</v>
+      </c>
+      <c r="C81" s="59">
+        <f>C70+C79</f>
+        <v>4.9260842623449577</v>
+      </c>
+    </row>
+    <row r="82" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="G83" s="51"/>
+      <c r="H83" s="52"/>
+      <c r="K83" t="s">
+        <v>41</v>
+      </c>
+      <c r="L83" s="29">
+        <v>8</v>
+      </c>
+      <c r="M83" s="30">
+        <v>8</v>
+      </c>
+      <c r="N83" s="31">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="L84" s="32">
+        <v>8</v>
+      </c>
+      <c r="M84" s="33">
+        <v>8.0749999999999993</v>
+      </c>
+      <c r="N84" s="34">
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="85" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L85" s="35">
+        <v>57</v>
+      </c>
+      <c r="M85" s="36">
+        <v>56.25</v>
+      </c>
+      <c r="N85" s="37">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="88" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K89" t="s">
+        <v>40</v>
+      </c>
+      <c r="L89" s="47">
+        <v>1</v>
+      </c>
+      <c r="M89" s="53">
+        <v>1</v>
+      </c>
+      <c r="N89" s="48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I91" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I92" s="49">
+        <v>1</v>
+      </c>
+      <c r="K92" t="s">
+        <v>42</v>
+      </c>
+      <c r="L92" s="38" cm="1">
+        <f t="array" ref="L92:N94">MINVERSE(L83:N85)</f>
+        <v>35.384735202492791</v>
+      </c>
+      <c r="M92" s="39">
+        <v>-26.137071651090803</v>
+      </c>
+      <c r="N92" s="40">
+        <v>-1.2803738317757178</v>
+      </c>
+    </row>
+    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="I93" s="54">
+        <v>1</v>
+      </c>
+      <c r="L93" s="41">
+        <v>-26.137071651090782</v>
+      </c>
+      <c r="M93" s="42">
+        <v>20.809968847352376</v>
+      </c>
+      <c r="N93" s="43">
+        <v>0.7476635514018819</v>
+      </c>
+    </row>
+    <row r="94" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I94" s="50">
+        <v>7</v>
+      </c>
+      <c r="L94" s="44">
+        <v>-1.2803738317757205</v>
+      </c>
+      <c r="M94" s="45">
+        <v>0.74766355140188456</v>
+      </c>
+      <c r="N94" s="46">
+        <v>7.4766355140187507E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K98" t="s">
+        <v>43</v>
+      </c>
+      <c r="L98" s="47" cm="1">
+        <f t="array" ref="L98">MMULT(L89:N89,L92:L94)</f>
+        <v>0.2850467289719667</v>
+      </c>
+      <c r="M98" s="53" cm="1">
+        <f t="array" ref="M98">MMULT(L89:N89,M92:M94)</f>
+        <v>-9.3457943925234765E-2</v>
+      </c>
+      <c r="N98" s="48" cm="1">
+        <f t="array" ref="N98">MMULT(L89:N89,N92:N94)</f>
+        <v>-9.3457943925233655E-3</v>
+      </c>
+    </row>
+    <row r="101" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K102" t="s">
+        <v>44</v>
+      </c>
+      <c r="L102" s="55" cm="1">
+        <f t="array" ref="L102">MMULT(L98:N98,I92:I94)</f>
+        <v>0.12616822429906838</v>
+      </c>
+    </row>
+    <row r="103" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="11:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K104" t="s">
+        <v>45</v>
+      </c>
+      <c r="L104" s="55">
+        <f>(1+L102)^0.5</f>
+        <v>1.0612107351035742</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="B15:F15"/>
     <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B80:C80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFB40B9-7D53-4AA7-907A-A9AEE21FBC2F}">
+  <dimension ref="A4:I79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="29">
+        <v>161</v>
+      </c>
+      <c r="C5" s="30">
+        <v>123</v>
+      </c>
+      <c r="D5" s="31">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="32">
+        <v>2120</v>
+      </c>
+      <c r="C6" s="33">
+        <v>1635</v>
+      </c>
+      <c r="D6" s="34">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="35">
+        <v>2082</v>
+      </c>
+      <c r="C7" s="36">
+        <v>1591</v>
+      </c>
+      <c r="D7" s="37">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="29">
+        <v>10</v>
+      </c>
+      <c r="C13" s="30">
+        <v>123</v>
+      </c>
+      <c r="D13" s="31">
+        <v>138</v>
+      </c>
+      <c r="G13" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="55">
+        <f>MDETERM(B13:D15)</f>
+        <v>62126.000000000291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="32">
+        <v>123</v>
+      </c>
+      <c r="C14" s="33">
+        <v>1635</v>
+      </c>
+      <c r="D14" s="34">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="35">
+        <v>138</v>
+      </c>
+      <c r="C15" s="36">
+        <v>1591</v>
+      </c>
+      <c r="D15" s="37">
+        <v>2048</v>
+      </c>
+      <c r="G15" t="s">
+        <v>52</v>
+      </c>
+      <c r="H15" s="55">
+        <f>MDETERM(B5:D7)/H13</f>
+        <v>10.731175353314267</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19" s="29">
+        <v>10</v>
+      </c>
+      <c r="C19" s="30">
+        <v>123</v>
+      </c>
+      <c r="D19" s="31">
+        <v>161</v>
+      </c>
+      <c r="G19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="55">
+        <f>MDETERM(B19:D21)/H13</f>
+        <v>-0.35500434600649744</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="32">
+        <v>123</v>
+      </c>
+      <c r="C20" s="33">
+        <v>1635</v>
+      </c>
+      <c r="D20" s="34">
+        <v>2120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="35">
+        <v>138</v>
+      </c>
+      <c r="C21" s="36">
+        <v>1591</v>
+      </c>
+      <c r="D21" s="37">
+        <v>2082</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" s="29">
+        <v>10</v>
+      </c>
+      <c r="C25" s="30">
+        <v>161</v>
+      </c>
+      <c r="D25" s="31">
+        <v>138</v>
+      </c>
+      <c r="G25" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="55">
+        <f>MDETERM(B25:D27)/H13</f>
+        <v>0.83478736760777084</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="32">
+        <v>123</v>
+      </c>
+      <c r="C26" s="33">
+        <v>2120</v>
+      </c>
+      <c r="D26" s="34">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="35">
+        <v>138</v>
+      </c>
+      <c r="C27" s="36">
+        <v>2082</v>
+      </c>
+      <c r="D27" s="37">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C41" s="29">
+        <v>1</v>
+      </c>
+      <c r="D41" s="30">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="E41" s="31">
+        <v>-0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="32">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="D42" s="33">
+        <v>1</v>
+      </c>
+      <c r="E42" s="34">
+        <v>-0.80300000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>2</v>
+      </c>
+      <c r="C43" s="35">
+        <v>-0.88200000000000001</v>
+      </c>
+      <c r="D43" s="36">
+        <v>-0.80300000000000005</v>
+      </c>
+      <c r="E43" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
+        <v>60</v>
+      </c>
+      <c r="G47">
+        <f>MDETERM(C41:E43)</f>
+        <v>1.7497352000000011E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48">
+        <f>MDETERM(D42:E43)</f>
+        <v>0.35519099999999992</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51">
+        <f>1-G47/G48</f>
+        <v>0.95073818874915184</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>63</v>
+      </c>
+      <c r="F54" t="s">
+        <v>62</v>
+      </c>
+      <c r="G54">
+        <f>1-(1-G51)*(10-1)/(10-2-1)</f>
+        <v>0.9366633855346238</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="61"/>
+    </row>
+    <row r="61" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="29">
+        <v>1</v>
+      </c>
+      <c r="D62" s="31">
+        <v>-0.80300000000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="35">
+        <v>-0.80300000000000005</v>
+      </c>
+      <c r="D63" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C66" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D66" s="48">
+        <f>MDETERM(C62:D63)</f>
+        <v>0.35519099999999992</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C69" s="29">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="D69" s="31">
+        <v>-0.80300000000000005</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="35">
+        <v>-0.88200000000000001</v>
+      </c>
+      <c r="D70" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D72" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="E72" s="48">
+        <f>MDETERM(C69:D70)</f>
+        <v>0.24775399999999995</v>
+      </c>
+      <c r="H72" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="I72" s="48">
+        <f>E72/D66</f>
+        <v>0.69752330436300469</v>
+      </c>
+    </row>
+    <row r="74" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C75" s="29">
+        <v>1</v>
+      </c>
+      <c r="D75" s="31">
+        <v>0.95599999999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="35">
+        <v>-0.80300000000000005</v>
+      </c>
+      <c r="D76" s="37">
+        <v>-0.88200000000000001</v>
+      </c>
+    </row>
+    <row r="78" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D79" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E79" s="48">
+        <f>MDETERM(C75:D76)</f>
+        <v>-0.11433199999999999</v>
+      </c>
+      <c r="H79" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="I79" s="48">
+        <f>E79/D66</f>
+        <v>-0.32188878659650727</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add `task-5` in `econometrics`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/econometrics/task-3/task-3.xlsx
+++ b/3-course-6-semester/econometrics/task-3/task-3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\econometrics\task-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mag\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4C83AD-B1FE-4ACD-AEB3-A25B60DFF485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD9587B-D1D3-4F0F-88D3-630B633BF7DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ДЗ №3" sheetId="1" r:id="rId1"/>
@@ -25,34 +25,24 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
       <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+        <ext xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray" uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
           <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
         </ext>
       </extLst>
@@ -834,33 +824,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -893,16 +856,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1550,8 +1540,8 @@
       <xdr:row>56</xdr:row>
       <xdr:rowOff>105834</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -1632,31 +1622,7 @@
                       <a:ea typeface="+mn-ea"/>
                       <a:cs typeface="+mn-cs"/>
                     </a:rPr>
-                    <m:t>=7.56</m:t>
-                  </m:r>
-                  <m:r>
-                    <a:rPr lang="en-US" sz="1400" b="0" i="1">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1"/>
-                      </a:solidFill>
-                      <a:effectLst/>
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:rPr>
-                    <m:t>−</m:t>
-                  </m:r>
-                  <m:r>
-                    <a:rPr lang="ru-RU" sz="1400" b="0" i="1">
-                      <a:solidFill>
-                        <a:schemeClr val="dk1"/>
-                      </a:solidFill>
-                      <a:effectLst/>
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:rPr>
-                    <m:t>4.67</m:t>
+                    <m:t>=7.56−4.67</m:t>
                   </m:r>
                   <m:sSub>
                     <m:sSubPr>
@@ -1801,7 +1767,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="TextBox 3">
@@ -3049,8 +3015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R104"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P84" sqref="P84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,13 +3185,13 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="21"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
       <c r="J13" s="13" t="s">
         <v>12</v>
       </c>
@@ -3234,13 +3200,13 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="24"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="56"/>
       <c r="J14" s="13" t="s">
         <v>13</v>
       </c>
@@ -3249,13 +3215,13 @@
       </c>
     </row>
     <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="24"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
       <c r="J15" s="14" t="s">
         <v>14</v>
       </c>
@@ -3264,13 +3230,13 @@
       </c>
     </row>
     <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
+      <c r="C16" s="58"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
     </row>
     <row r="17" spans="10:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
@@ -3444,7 +3410,7 @@
       <c r="M26" s="13">
         <v>2.524944190751977</v>
       </c>
-      <c r="N26" s="28">
+      <c r="N26" s="19">
         <v>6.5013524286557031E-2</v>
       </c>
       <c r="O26" s="13">
@@ -3845,10 +3811,10 @@
       </c>
     </row>
     <row r="70" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="47" t="s">
+      <c r="B70" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="C70" s="48">
+      <c r="C70" s="39">
         <f>K63+K64*1+K65*7</f>
         <v>4.1892523364485985</v>
       </c>
@@ -3981,123 +3947,127 @@
       </c>
     </row>
     <row r="80" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B80" s="56" t="s">
+      <c r="B80" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="57"/>
-    </row>
-    <row r="81" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B81" s="58">
+      <c r="C80" s="61"/>
+    </row>
+    <row r="81" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B81" s="47">
         <f>C70-C79</f>
         <v>3.4524204105522398</v>
       </c>
-      <c r="C81" s="59">
+      <c r="C81" s="48">
         <f>C70+C79</f>
         <v>4.9260842623449577</v>
       </c>
     </row>
-    <row r="82" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="83" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G83" s="51"/>
-      <c r="H83" s="52"/>
+    <row r="82" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="83" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="G83" s="42"/>
+      <c r="H83" s="43"/>
       <c r="K83" t="s">
         <v>41</v>
       </c>
-      <c r="L83" s="29">
+      <c r="L83" s="20">
         <v>8</v>
       </c>
-      <c r="M83" s="30">
+      <c r="M83" s="21">
         <v>8</v>
       </c>
-      <c r="N83" s="31">
+      <c r="N83" s="22">
         <v>57</v>
       </c>
-    </row>
-    <row r="84" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="L84" s="32">
+      <c r="Q83">
+        <f>MMULT(I92:I94,L89:N89)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="L84" s="23">
         <v>8</v>
       </c>
-      <c r="M84" s="33">
+      <c r="M84" s="24">
         <v>8.0749999999999993</v>
       </c>
-      <c r="N84" s="34">
+      <c r="N84" s="25">
         <v>56.25</v>
       </c>
     </row>
-    <row r="85" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="L85" s="35">
+    <row r="85" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L85" s="26">
         <v>57</v>
       </c>
-      <c r="M85" s="36">
+      <c r="M85" s="27">
         <v>56.25</v>
       </c>
-      <c r="N85" s="37">
+      <c r="N85" s="28">
         <v>427</v>
       </c>
     </row>
-    <row r="88" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K89" t="s">
         <v>40</v>
       </c>
-      <c r="L89" s="47">
+      <c r="L89" s="38">
         <v>1</v>
       </c>
-      <c r="M89" s="53">
+      <c r="M89" s="44">
         <v>1</v>
       </c>
-      <c r="N89" s="48">
+      <c r="N89" s="39">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I91" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="92" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I92" s="49">
+    <row r="92" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I92" s="40">
         <v>1</v>
       </c>
       <c r="K92" t="s">
         <v>42</v>
       </c>
-      <c r="L92" s="38" cm="1">
+      <c r="L92" s="29" cm="1">
         <f t="array" ref="L92:N94">MINVERSE(L83:N85)</f>
         <v>35.384735202492791</v>
       </c>
-      <c r="M92" s="39">
+      <c r="M92" s="30">
         <v>-26.137071651090803</v>
       </c>
-      <c r="N92" s="40">
+      <c r="N92" s="31">
         <v>-1.2803738317757178</v>
       </c>
     </row>
-    <row r="93" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="I93" s="54">
+    <row r="93" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="I93" s="45">
         <v>1</v>
       </c>
-      <c r="L93" s="41">
+      <c r="L93" s="32">
         <v>-26.137071651090782</v>
       </c>
-      <c r="M93" s="42">
+      <c r="M93" s="33">
         <v>20.809968847352376</v>
       </c>
-      <c r="N93" s="43">
+      <c r="N93" s="34">
         <v>0.7476635514018819</v>
       </c>
     </row>
-    <row r="94" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I94" s="50">
+    <row r="94" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I94" s="41">
         <v>7</v>
       </c>
-      <c r="L94" s="44">
+      <c r="L94" s="35">
         <v>-1.2803738317757205</v>
       </c>
-      <c r="M94" s="45">
+      <c r="M94" s="36">
         <v>0.74766355140188456</v>
       </c>
-      <c r="N94" s="46">
+      <c r="N94" s="37">
         <v>7.4766355140187507E-2</v>
       </c>
     </row>
@@ -4106,15 +4076,15 @@
       <c r="K98" t="s">
         <v>43</v>
       </c>
-      <c r="L98" s="47" cm="1">
+      <c r="L98" s="38" cm="1">
         <f t="array" ref="L98">MMULT(L89:N89,L92:L94)</f>
         <v>0.2850467289719667</v>
       </c>
-      <c r="M98" s="53" cm="1">
+      <c r="M98" s="44" cm="1">
         <f t="array" ref="M98">MMULT(L89:N89,M92:M94)</f>
         <v>-9.3457943925234765E-2</v>
       </c>
-      <c r="N98" s="48" cm="1">
+      <c r="N98" s="39" cm="1">
         <f t="array" ref="N98">MMULT(L89:N89,N92:N94)</f>
         <v>-9.3457943925233655E-3</v>
       </c>
@@ -4124,7 +4094,7 @@
       <c r="K102" t="s">
         <v>44</v>
       </c>
-      <c r="L102" s="55" cm="1">
+      <c r="L102" s="46" cm="1">
         <f t="array" ref="L102">MMULT(L98:N98,I92:I94)</f>
         <v>0.12616822429906838</v>
       </c>
@@ -4134,7 +4104,7 @@
       <c r="K104" t="s">
         <v>45</v>
       </c>
-      <c r="L104" s="55">
+      <c r="L104" s="46">
         <f>(1+L102)^0.5</f>
         <v>1.0612107351035742</v>
       </c>
@@ -4156,7 +4126,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FFB40B9-7D53-4AA7-907A-A9AEE21FBC2F}">
   <dimension ref="A4:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
@@ -4167,38 +4137,38 @@
   <sheetData>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="29">
+      <c r="B5" s="20">
         <v>161</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="21">
         <v>123</v>
       </c>
-      <c r="D5" s="31">
+      <c r="D5" s="22">
         <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="32">
+      <c r="B6" s="23">
         <v>2120</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="24">
         <v>1635</v>
       </c>
-      <c r="D6" s="34">
+      <c r="D6" s="25">
         <v>1591</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="35">
+      <c r="B7" s="26">
         <v>2082</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="27">
         <v>1591</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="28">
         <v>2048</v>
       </c>
     </row>
@@ -4208,137 +4178,137 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="29">
+      <c r="B13" s="20">
         <v>10</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="21">
         <v>123</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="22">
         <v>138</v>
       </c>
       <c r="G13" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="55">
+      <c r="H13" s="46">
         <f>MDETERM(B13:D15)</f>
         <v>62126.000000000291</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="32">
+      <c r="B14" s="23">
         <v>123</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="24">
         <v>1635</v>
       </c>
-      <c r="D14" s="34">
+      <c r="D14" s="25">
         <v>1591</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="35">
+      <c r="B15" s="26">
         <v>138</v>
       </c>
-      <c r="C15" s="36">
+      <c r="C15" s="27">
         <v>1591</v>
       </c>
-      <c r="D15" s="37">
+      <c r="D15" s="28">
         <v>2048</v>
       </c>
       <c r="G15" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="55">
+      <c r="H15" s="46">
         <f>MDETERM(B5:D7)/H13</f>
         <v>10.731175353314267</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="20">
         <v>10</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="21">
         <v>123</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="22">
         <v>161</v>
       </c>
       <c r="G19" t="s">
         <v>53</v>
       </c>
-      <c r="H19" s="55">
+      <c r="H19" s="46">
         <f>MDETERM(B19:D21)/H13</f>
         <v>-0.35500434600649744</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="32">
+      <c r="B20" s="23">
         <v>123</v>
       </c>
-      <c r="C20" s="33">
+      <c r="C20" s="24">
         <v>1635</v>
       </c>
-      <c r="D20" s="34">
+      <c r="D20" s="25">
         <v>2120</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="35">
+      <c r="B21" s="26">
         <v>138</v>
       </c>
-      <c r="C21" s="36">
+      <c r="C21" s="27">
         <v>1591</v>
       </c>
-      <c r="D21" s="37">
+      <c r="D21" s="28">
         <v>2082</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="B25" s="29">
+      <c r="B25" s="20">
         <v>10</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="21">
         <v>161</v>
       </c>
-      <c r="D25" s="31">
+      <c r="D25" s="22">
         <v>138</v>
       </c>
       <c r="G25" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="55">
+      <c r="H25" s="46">
         <f>MDETERM(B25:D27)/H13</f>
         <v>0.83478736760777084</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="32">
+      <c r="B26" s="23">
         <v>123</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="24">
         <v>2120</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="25">
         <v>1591</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="35">
+      <c r="B27" s="26">
         <v>138</v>
       </c>
-      <c r="C27" s="36">
+      <c r="C27" s="27">
         <v>2082</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D27" s="28">
         <v>2048</v>
       </c>
     </row>
@@ -4360,13 +4330,13 @@
       <c r="B41" t="s">
         <v>0</v>
       </c>
-      <c r="C41" s="29">
+      <c r="C41" s="20">
         <v>1</v>
       </c>
-      <c r="D41" s="30">
+      <c r="D41" s="21">
         <v>0.95599999999999996</v>
       </c>
-      <c r="E41" s="31">
+      <c r="E41" s="22">
         <v>-0.88200000000000001</v>
       </c>
     </row>
@@ -4374,13 +4344,13 @@
       <c r="B42" t="s">
         <v>1</v>
       </c>
-      <c r="C42" s="32">
+      <c r="C42" s="23">
         <v>0.95599999999999996</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D42" s="24">
         <v>1</v>
       </c>
-      <c r="E42" s="34">
+      <c r="E42" s="25">
         <v>-0.80300000000000005</v>
       </c>
     </row>
@@ -4388,13 +4358,13 @@
       <c r="B43" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="35">
+      <c r="C43" s="26">
         <v>-0.88200000000000001</v>
       </c>
-      <c r="D43" s="36">
+      <c r="D43" s="27">
         <v>-0.80300000000000005</v>
       </c>
-      <c r="E43" s="37">
+      <c r="E43" s="28">
         <v>1</v>
       </c>
     </row>
@@ -4438,99 +4408,99 @@
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C55" s="61"/>
+      <c r="C55" s="50"/>
     </row>
     <row r="61" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="29">
+      <c r="C62" s="20">
         <v>1</v>
       </c>
-      <c r="D62" s="31">
+      <c r="D62" s="22">
         <v>-0.80300000000000005</v>
       </c>
     </row>
     <row r="63" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="35">
+      <c r="C63" s="26">
         <v>-0.80300000000000005</v>
       </c>
-      <c r="D63" s="37">
+      <c r="D63" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="65" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="66" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C66" s="47" t="s">
+      <c r="C66" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="D66" s="48">
+      <c r="D66" s="39">
         <f>MDETERM(C62:D63)</f>
         <v>0.35519099999999992</v>
       </c>
     </row>
     <row r="68" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C69" s="29">
+      <c r="C69" s="20">
         <v>0.95599999999999996</v>
       </c>
-      <c r="D69" s="31">
+      <c r="D69" s="22">
         <v>-0.80300000000000005</v>
       </c>
     </row>
     <row r="70" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C70" s="35">
+      <c r="C70" s="26">
         <v>-0.88200000000000001</v>
       </c>
-      <c r="D70" s="37">
+      <c r="D70" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="72" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D72" s="47" t="s">
+      <c r="D72" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="E72" s="48">
+      <c r="E72" s="39">
         <f>MDETERM(C69:D70)</f>
         <v>0.24775399999999995</v>
       </c>
-      <c r="H72" s="47" t="s">
+      <c r="H72" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="I72" s="48">
+      <c r="I72" s="39">
         <f>E72/D66</f>
         <v>0.69752330436300469</v>
       </c>
     </row>
     <row r="74" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="75" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C75" s="29">
+      <c r="C75" s="20">
         <v>1</v>
       </c>
-      <c r="D75" s="31">
+      <c r="D75" s="22">
         <v>0.95599999999999996</v>
       </c>
     </row>
     <row r="76" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C76" s="35">
+      <c r="C76" s="26">
         <v>-0.80300000000000005</v>
       </c>
-      <c r="D76" s="37">
+      <c r="D76" s="28">
         <v>-0.88200000000000001</v>
       </c>
     </row>
     <row r="78" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="79" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D79" s="47" t="s">
+      <c r="D79" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="E79" s="48">
+      <c r="E79" s="39">
         <f>MDETERM(C75:D76)</f>
         <v>-0.11433199999999999</v>
       </c>
-      <c r="H79" s="47" t="s">
+      <c r="H79" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="I79" s="48">
+      <c r="I79" s="39">
         <f>E79/D66</f>
         <v>-0.32188878659650727</v>
       </c>

</xml_diff>